<commit_message>
update location api code
</commit_message>
<xml_diff>
--- a/EWB Masterfile Build-Up - as 12.12.2022.xlsx
+++ b/EWB Masterfile Build-Up - as 12.12.2022.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SuperSam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\T\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11531" uniqueCount="1722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11539" uniqueCount="1730">
   <si>
     <t>DBCode</t>
   </si>
@@ -5207,6 +5207,30 @@
   </si>
   <si>
     <t>select NewID() Id,c.Id CompanyId,a.BankName,'','','Savings',a.AccountNumber,a.BranchCode,'Select Signatories',a.Signatory1,a.Signatory1,'Default','system',getdate(),'system',getdate()</t>
+  </si>
+  <si>
+    <t>use [FAS_Live]</t>
+  </si>
+  <si>
+    <t>Update [dbo].[Bank] set Signatory2 = Signatory2_2</t>
+  </si>
+  <si>
+    <t>from (Select c.Id CompanyId2, a.Signatory2 Signatory2_2,a.BankName BankName2 from #TempBank as a</t>
+  </si>
+  <si>
+    <t>INNER JOIN dbo.DatabaseConnectionSetup as b on a.DBCode = b.Code</t>
+  </si>
+  <si>
+    <t>INNER JOIN  dbo.Company as c on convert(int,a.EntityCode) =  convert(int,c.Code) and b.Id  = c.DatabaseConnectionSetupId</t>
+  </si>
+  <si>
+    <t>where IsNumeric(c.Code) = 1) as b</t>
+  </si>
+  <si>
+    <t>where CompanyId = CompanyId2 and BankName2 = BankName</t>
+  </si>
+  <si>
+    <t>---Fix Signatory</t>
   </si>
 </sst>
 </file>
@@ -5284,7 +5308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5298,6 +5322,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5578,20 +5603,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I4" sqref="I4:I33"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.140625" style="6" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
@@ -43318,10 +43343,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A31"/>
+  <dimension ref="A2:A44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43446,6 +43471,46 @@
         <v>1704</v>
       </c>
     </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1728</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>